<commit_message>
generate account; cancle ad download
</commit_message>
<xml_diff>
--- a/BitherX.xlsx
+++ b/BitherX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" tabRatio="449"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="112">
   <si>
     <t>冷钱包</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -298,13 +298,469 @@
   </si>
   <si>
     <t>EncryptedData</t>
+  </si>
+  <si>
+    <t>HDAccount</t>
+  </si>
+  <si>
+    <t>MnemonicCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>initHDAccount()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EncryptedData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeterministicKey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDKeyDerivation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ECKey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDAccount.HDAccountAddress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.生成椭圆曲线密钥对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.加密私钥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.生成Address对象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ECKeyPairGenerator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ECKeyGenerationParameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ECPrivateKeyParameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ECPublicKeyParameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KeyCrypterScrypt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>ECKey.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>generateECKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(xRandom)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PrivateKeyUtil.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>encrypt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(ecKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>password)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AsymmetricCipherKeyPair[非对称密钥对]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MnemonicCodeAndroid</t>
+  </si>
+  <si>
+    <t>1.生成种子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.生成主账户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.加密HD账户种子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.加密记忆种子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.生成椭圆曲线密钥对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.生成记忆种子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>random.nextBytes(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>mnemonicSeed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>2.生成HD种子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>mnemonicCode.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>toSeed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(mnemonicCode.toMnemonic(mnemonicSeed)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>""</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>5.生成主账户私钥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.初始化HD账户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A.生成椭圆曲线密钥对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B.root账户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C.子账户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>DeterministicKey master = HDKeyDerivation.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>createMasterPrivateKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>hdSeed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ECKey(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>mnemonicSeed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mnemonicSeed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>new byte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +793,52 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FFCC7832"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF660E7A"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF000080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF0000FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -366,7 +868,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -377,6 +879,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -673,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:W73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
+      <selection activeCell="Q73" sqref="Q73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -686,8 +1191,11 @@
     <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="13.75" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="9" max="9" width="10.625" customWidth="1"/>
     <col min="11" max="11" width="11.25" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="10.375" customWidth="1"/>
+    <col min="21" max="21" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -958,48 +1466,81 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:23">
       <c r="L33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:23">
       <c r="K34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:23">
       <c r="K35" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:23">
       <c r="K36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:23" ht="18">
       <c r="A43" t="s">
         <v>57</v>
       </c>
       <c r="B43" t="s">
         <v>58</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="C44" t="s">
+      <c r="F43" t="s">
+        <v>83</v>
+      </c>
+      <c r="I43" t="s">
+        <v>91</v>
+      </c>
+      <c r="M43" t="s">
+        <v>86</v>
+      </c>
+      <c r="O43" t="s">
+        <v>87</v>
+      </c>
+      <c r="R43" t="s">
+        <v>93</v>
+      </c>
+      <c r="U43" t="s">
+        <v>88</v>
+      </c>
+      <c r="W43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="18">
+      <c r="C44" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="F44" t="s">
+        <v>84</v>
+      </c>
+      <c r="I44" t="s">
+        <v>92</v>
+      </c>
+      <c r="N44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
       <c r="C45" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="F45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23">
       <c r="C46" t="s">
         <v>62</v>
       </c>
@@ -1007,40 +1548,55 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:23">
       <c r="D47" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:23">
       <c r="C48" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="2:11">
       <c r="B50" t="s">
         <v>66</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="51" spans="2:7">
+      <c r="J50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11">
       <c r="D51" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="52" spans="2:7">
+      <c r="E51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11">
       <c r="E52" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="53" spans="2:7">
+      <c r="J52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11">
       <c r="E53" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="54" spans="2:7">
+      <c r="J53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11">
       <c r="D54" t="s">
         <v>71</v>
       </c>
@@ -1050,25 +1606,134 @@
       <c r="G54" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="55" spans="2:7">
+      <c r="J54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11">
       <c r="D55" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:11">
       <c r="D56" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:11">
       <c r="D57" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="2:11">
       <c r="D58" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11">
+      <c r="C60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" ht="18">
+      <c r="C61" s="4"/>
+      <c r="D61" t="s">
+        <v>71</v>
+      </c>
+      <c r="K61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" ht="18">
+      <c r="C62" s="4"/>
+      <c r="D62" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" t="s">
+        <v>69</v>
+      </c>
+      <c r="K62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" ht="18">
+      <c r="D63" s="4"/>
+      <c r="E63" t="s">
+        <v>70</v>
+      </c>
+      <c r="J63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" ht="18">
+      <c r="D64" t="s">
+        <v>78</v>
+      </c>
+      <c r="K64" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="4:12">
+      <c r="D65" t="s">
+        <v>79</v>
+      </c>
+      <c r="J65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="4:12">
+      <c r="D66" t="s">
+        <v>80</v>
+      </c>
+      <c r="J66" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="4:12">
+      <c r="D67" t="s">
+        <v>77</v>
+      </c>
+      <c r="J67" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="4:12" ht="18">
+      <c r="E68" t="s">
+        <v>81</v>
+      </c>
+      <c r="K68" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="4:12">
+      <c r="E69" t="s">
+        <v>82</v>
+      </c>
+      <c r="J69" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="4:12">
+      <c r="K70" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="71" spans="4:12" ht="18">
+      <c r="L71" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="4:12">
+      <c r="K72" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="4:12">
+      <c r="K73" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
account details ; enter activity direct without wait for blocks download
</commit_message>
<xml_diff>
--- a/BitherX.xlsx
+++ b/BitherX.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="122">
   <si>
     <t>冷钱包</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -753,6 +753,46 @@
       </rPr>
       <t xml:space="preserve">; </t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通账户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成账户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看私钥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看BIP38私钥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>签名消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HD账户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看密语</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看xPubB58密语</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1178,17 +1218,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W73"/>
+  <dimension ref="A1:W89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
-      <selection activeCell="Q73" sqref="Q73"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="11.875" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
     <col min="4" max="4" width="13.75" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
     <col min="9" max="9" width="10.625" customWidth="1"/>
@@ -1734,6 +1774,55 @@
     <row r="73" spans="4:12">
       <c r="K73" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>112</v>
+      </c>
+      <c r="B81" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="C82" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="C83" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="C84" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="B86" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="C87" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="C88" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="C89" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>